<commit_message>
Sayfa Adı olmayan dosyalar için kod güncellendi
</commit_message>
<xml_diff>
--- a/D2.xlsx
+++ b/D2.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sayfa1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sayfa11" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Sayfa2" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Sayfa3" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Sayfa4" sheetId="4" state="visible" r:id="rId6"/>
@@ -509,38 +509,38 @@
       </c>
       <c r="I5" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J5" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K5" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L5" s="12" t="str">
         <f aca="false">I5&amp;"."&amp;J5&amp;"."&amp;K5</f>
-        <v>6.9.2022</v>
+        <v>3.11.2022</v>
       </c>
       <c r="M5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>1114</v>
+        <v>5356</v>
       </c>
       <c r="N5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>13951</v>
+        <v>14233</v>
       </c>
       <c r="O5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8990</v>
+        <v>9349</v>
       </c>
       <c r="P5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15481</v>
+        <v>24498</v>
       </c>
       <c r="Q5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29489</v>
+        <v>12469</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -564,38 +564,38 @@
       </c>
       <c r="I6" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J6" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K6" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L6" s="12" t="str">
         <f aca="false">I6&amp;"."&amp;J6&amp;"."&amp;K6</f>
-        <v>9.6.2022</v>
+        <v>10.3.2022</v>
       </c>
       <c r="M6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17345</v>
+        <v>29462</v>
       </c>
       <c r="N6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22034</v>
+        <v>8092</v>
       </c>
       <c r="O6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28274</v>
+        <v>19438</v>
       </c>
       <c r="P6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5132</v>
+        <v>17905</v>
       </c>
       <c r="Q6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17157</v>
+        <v>29202</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -619,38 +619,38 @@
       </c>
       <c r="I7" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J7" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K7" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L7" s="12" t="str">
         <f aca="false">I7&amp;"."&amp;J7&amp;"."&amp;K7</f>
-        <v>9.10.2022</v>
+        <v>1.5.2022</v>
       </c>
       <c r="M7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>1722</v>
+        <v>14763</v>
       </c>
       <c r="N7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>1800</v>
+        <v>21637</v>
       </c>
       <c r="O7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3787</v>
+        <v>24267</v>
       </c>
       <c r="P7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6884</v>
+        <v>23322</v>
       </c>
       <c r="Q7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2963</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -674,7 +674,7 @@
       </c>
       <c r="I8" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J8" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -685,27 +685,27 @@
       </c>
       <c r="L8" s="12" t="str">
         <f aca="false">I8&amp;"."&amp;J8&amp;"."&amp;K8</f>
-        <v>10.2.2022</v>
+        <v>7.2.2022</v>
       </c>
       <c r="M8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21140</v>
+        <v>24701</v>
       </c>
       <c r="N8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11592</v>
+        <v>18113</v>
       </c>
       <c r="O8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10616</v>
+        <v>6603</v>
       </c>
       <c r="P8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5499</v>
+        <v>9820</v>
       </c>
       <c r="Q8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4573</v>
+        <v>13292</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -729,38 +729,38 @@
       </c>
       <c r="I9" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J9" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K9" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L9" s="12" t="str">
         <f aca="false">I9&amp;"."&amp;J9&amp;"."&amp;K9</f>
-        <v>3.5.2022</v>
+        <v>2.8.2022</v>
       </c>
       <c r="M9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11202</v>
+        <v>29750</v>
       </c>
       <c r="N9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5935</v>
+        <v>8797</v>
       </c>
       <c r="O9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2768</v>
+        <v>14402</v>
       </c>
       <c r="P9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29397</v>
+        <v>20116</v>
       </c>
       <c r="Q9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23495</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -784,38 +784,38 @@
       </c>
       <c r="I10" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J10" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K10" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L10" s="12" t="str">
         <f aca="false">I10&amp;"."&amp;J10&amp;"."&amp;K10</f>
-        <v>5.8.2022</v>
+        <v>3.2.2022</v>
       </c>
       <c r="M10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23686</v>
+        <v>22038</v>
       </c>
       <c r="N10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2040</v>
+        <v>2944</v>
       </c>
       <c r="O10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9752</v>
+        <v>24185</v>
       </c>
       <c r="P10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22325</v>
+        <v>5190</v>
       </c>
       <c r="Q10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9768</v>
+        <v>13461</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -839,38 +839,38 @@
       </c>
       <c r="I11" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J11" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K11" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L11" s="12" t="str">
         <f aca="false">I11&amp;"."&amp;J11&amp;"."&amp;K11</f>
-        <v>5.5.2022</v>
+        <v>4.7.2022</v>
       </c>
       <c r="M11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23475</v>
+        <v>1988</v>
       </c>
       <c r="N11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10004</v>
+        <v>9046</v>
       </c>
       <c r="O11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9710</v>
+        <v>8104</v>
       </c>
       <c r="P11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21250</v>
+        <v>14502</v>
       </c>
       <c r="Q11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24712</v>
+        <v>8776</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1027,34 +1027,34 @@
       </c>
       <c r="J17" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K17" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L17" s="12" t="str">
         <f aca="false">I17&amp;"."&amp;J17&amp;"."&amp;K17</f>
-        <v>10.4.2022</v>
+        <v>10.10.2022</v>
       </c>
       <c r="M17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7193</v>
+        <v>24120</v>
       </c>
       <c r="N17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>13418</v>
+        <v>7007</v>
       </c>
       <c r="O17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>1584</v>
+        <v>27303</v>
       </c>
       <c r="P17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>12075</v>
+        <v>16844</v>
       </c>
       <c r="Q17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>604</v>
+        <v>22083</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1078,38 +1078,38 @@
       </c>
       <c r="I18" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J18" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K18" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L18" s="12" t="str">
         <f aca="false">I18&amp;"."&amp;J18&amp;"."&amp;K18</f>
-        <v>7.12.2022</v>
+        <v>4.10.2022</v>
       </c>
       <c r="M18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24257</v>
+        <v>7620</v>
       </c>
       <c r="N18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4564</v>
+        <v>20583</v>
       </c>
       <c r="O18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5282</v>
+        <v>20264</v>
       </c>
       <c r="P18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21039</v>
+        <v>1404</v>
       </c>
       <c r="Q18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29753</v>
+        <v>8115</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1133,38 +1133,38 @@
       </c>
       <c r="I19" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J19" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K19" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L19" s="12" t="str">
         <f aca="false">I19&amp;"."&amp;J19&amp;"."&amp;K19</f>
-        <v>7.9.2022</v>
+        <v>3.10.2022</v>
       </c>
       <c r="M19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>27884</v>
+        <v>8818</v>
       </c>
       <c r="N19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23368</v>
+        <v>15081</v>
       </c>
       <c r="O19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2663</v>
+        <v>20239</v>
       </c>
       <c r="P19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>14262</v>
+        <v>24747</v>
       </c>
       <c r="Q19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>1656</v>
+        <v>10154</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1188,38 +1188,38 @@
       </c>
       <c r="I20" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J20" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K20" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L20" s="12" t="str">
         <f aca="false">I20&amp;"."&amp;J20&amp;"."&amp;K20</f>
-        <v>2.9.2022</v>
+        <v>3.7.2022</v>
       </c>
       <c r="M20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>486</v>
+        <v>1854</v>
       </c>
       <c r="N20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23739</v>
+        <v>22802</v>
       </c>
       <c r="O20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28572</v>
+        <v>19915</v>
       </c>
       <c r="P20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6034</v>
+        <v>8032</v>
       </c>
       <c r="Q20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23678</v>
+        <v>15305</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1243,38 +1243,38 @@
       </c>
       <c r="I21" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J21" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="K21" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L21" s="12" t="str">
         <f aca="false">I21&amp;"."&amp;J21&amp;"."&amp;K21</f>
-        <v>5.12.2022</v>
+        <v>10.4.2022</v>
       </c>
       <c r="M21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28027</v>
+        <v>20150</v>
       </c>
       <c r="N21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28060</v>
+        <v>238</v>
       </c>
       <c r="O21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17458</v>
+        <v>6203</v>
       </c>
       <c r="P21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8346</v>
+        <v>8754</v>
       </c>
       <c r="Q21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10851</v>
+        <v>18167</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1298,38 +1298,38 @@
       </c>
       <c r="I22" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J22" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K22" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L22" s="12" t="str">
         <f aca="false">I22&amp;"."&amp;J22&amp;"."&amp;K22</f>
-        <v>5.1.2022</v>
+        <v>10.8.2022</v>
       </c>
       <c r="M22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23746</v>
+        <v>19079</v>
       </c>
       <c r="N22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>27484</v>
+        <v>28710</v>
       </c>
       <c r="O22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8497</v>
+        <v>13101</v>
       </c>
       <c r="P22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7004</v>
+        <v>1241</v>
       </c>
       <c r="Q22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>18682</v>
+        <v>12424</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1353,38 +1353,38 @@
       </c>
       <c r="I23" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J23" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K23" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L23" s="12" t="str">
         <f aca="false">I23&amp;"."&amp;J23&amp;"."&amp;K23</f>
-        <v>9.8.2022</v>
+        <v>3.9.2022</v>
       </c>
       <c r="M23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24412</v>
+        <v>14035</v>
       </c>
       <c r="N23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6977</v>
+        <v>14047</v>
       </c>
       <c r="O23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20836</v>
+        <v>10392</v>
       </c>
       <c r="P23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20254</v>
+        <v>18361</v>
       </c>
       <c r="Q23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17056</v>
+        <v>29852</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
baslik fonk. dosya ismine gore duzenlendi
</commit_message>
<xml_diff>
--- a/D2.xlsx
+++ b/D2.xlsx
@@ -38,9 +38,6 @@
     <t xml:space="preserve">Tarih</t>
   </si>
   <si>
-    <t xml:space="preserve">Poz No 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Poz No 2</t>
   </si>
   <si>
@@ -51,6 +48,9 @@
   </si>
   <si>
     <t xml:space="preserve">Poz No 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poz No 1</t>
   </si>
   <si>
     <t xml:space="preserve">Yüklenici</t>
@@ -420,7 +420,7 @@
   <dimension ref="B1:Q38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -508,38 +508,38 @@
       </c>
       <c r="I5" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J5" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="K5" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L5" s="12" t="str">
         <f aca="false">I5&amp;"."&amp;J5&amp;"."&amp;K5</f>
-        <v>1.11.2022</v>
+        <v>4.4.2022</v>
       </c>
       <c r="M5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7234</v>
+        <v>27742</v>
       </c>
       <c r="N5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6179</v>
+        <v>3979</v>
       </c>
       <c r="O5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>18690</v>
+        <v>5472</v>
       </c>
       <c r="P5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9625</v>
+        <v>4993</v>
       </c>
       <c r="Q5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>12880</v>
+        <v>23422</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -563,38 +563,38 @@
       </c>
       <c r="I6" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J6" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K6" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L6" s="12" t="str">
         <f aca="false">I6&amp;"."&amp;J6&amp;"."&amp;K6</f>
-        <v>7.8.2022</v>
+        <v>2.4.2022</v>
       </c>
       <c r="M6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>14041</v>
+        <v>8030</v>
       </c>
       <c r="N6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>865</v>
+        <v>6366</v>
       </c>
       <c r="O6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>26875</v>
+        <v>27814</v>
       </c>
       <c r="P6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22491</v>
+        <v>6565</v>
       </c>
       <c r="Q6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17103</v>
+        <v>24161</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -618,38 +618,38 @@
       </c>
       <c r="I7" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J7" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K7" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L7" s="12" t="str">
         <f aca="false">I7&amp;"."&amp;J7&amp;"."&amp;K7</f>
-        <v>3.5.2022</v>
+        <v>2.4.2022</v>
       </c>
       <c r="M7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7311</v>
+        <v>23990</v>
       </c>
       <c r="N7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>25324</v>
+        <v>24735</v>
       </c>
       <c r="O7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24611</v>
+        <v>26327</v>
       </c>
       <c r="P7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17588</v>
+        <v>25753</v>
       </c>
       <c r="Q7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>18237</v>
+        <v>4942</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -673,38 +673,38 @@
       </c>
       <c r="I8" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J8" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="K8" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L8" s="12" t="str">
         <f aca="false">I8&amp;"."&amp;J8&amp;"."&amp;K8</f>
-        <v>9.11.2022</v>
+        <v>4.3.2022</v>
       </c>
       <c r="M8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20502</v>
+        <v>12421</v>
       </c>
       <c r="N8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28969</v>
+        <v>26490</v>
       </c>
       <c r="O8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10270</v>
+        <v>9700</v>
       </c>
       <c r="P8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>27172</v>
+        <v>6010</v>
       </c>
       <c r="Q8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17143</v>
+        <v>11654</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -728,38 +728,38 @@
       </c>
       <c r="I9" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J9" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="K9" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L9" s="12" t="str">
         <f aca="false">I9&amp;"."&amp;J9&amp;"."&amp;K9</f>
-        <v>5.9.2022</v>
+        <v>4.3.2022</v>
       </c>
       <c r="M9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>26619</v>
+        <v>26926</v>
       </c>
       <c r="N9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3275</v>
+        <v>23954</v>
       </c>
       <c r="O9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29003</v>
+        <v>26705</v>
       </c>
       <c r="P9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>14338</v>
+        <v>22961</v>
       </c>
       <c r="Q9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29930</v>
+        <v>2375</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -783,38 +783,38 @@
       </c>
       <c r="I10" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J10" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K10" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L10" s="12" t="str">
         <f aca="false">I10&amp;"."&amp;J10&amp;"."&amp;K10</f>
-        <v>9.1.2022</v>
+        <v>6.5.2022</v>
       </c>
       <c r="M10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20823</v>
+        <v>324</v>
       </c>
       <c r="N10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15605</v>
+        <v>23492</v>
       </c>
       <c r="O10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16526</v>
+        <v>8530</v>
       </c>
       <c r="P10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21729</v>
+        <v>12395</v>
       </c>
       <c r="Q10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>18723</v>
+        <v>5401</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -838,38 +838,38 @@
       </c>
       <c r="I11" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J11" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K11" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L11" s="12" t="str">
         <f aca="false">I11&amp;"."&amp;J11&amp;"."&amp;K11</f>
-        <v>10.6.2022</v>
+        <v>1.5.2022</v>
       </c>
       <c r="M11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>18578</v>
+        <v>11910</v>
       </c>
       <c r="N11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24233</v>
+        <v>6816</v>
       </c>
       <c r="O11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11091</v>
+        <v>9229</v>
       </c>
       <c r="P11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24254</v>
+        <v>8314</v>
       </c>
       <c r="Q11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23321</v>
+        <v>10693</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,38 +1022,38 @@
       </c>
       <c r="I17" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="J17" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K17" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L17" s="12" t="str">
         <f aca="false">I17&amp;"."&amp;J17&amp;"."&amp;K17</f>
-        <v>10.1.2022</v>
+        <v>6.5.2022</v>
       </c>
       <c r="M17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6836</v>
+        <v>26022</v>
       </c>
       <c r="N17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>25564</v>
+        <v>7899</v>
       </c>
       <c r="O17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8860</v>
+        <v>27178</v>
       </c>
       <c r="P17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15891</v>
+        <v>1910</v>
       </c>
       <c r="Q17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6563</v>
+        <v>18560</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1077,7 +1077,7 @@
       </c>
       <c r="I18" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="J18" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -1088,27 +1088,27 @@
       </c>
       <c r="L18" s="12" t="str">
         <f aca="false">I18&amp;"."&amp;J18&amp;"."&amp;K18</f>
-        <v>4.10.2022</v>
+        <v>9.10.2022</v>
       </c>
       <c r="M18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5210</v>
+        <v>16647</v>
       </c>
       <c r="N18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21759</v>
+        <v>22058</v>
       </c>
       <c r="O18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10779</v>
+        <v>24433</v>
       </c>
       <c r="P18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16468</v>
+        <v>25051</v>
       </c>
       <c r="Q18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24414</v>
+        <v>22312</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1132,38 +1132,38 @@
       </c>
       <c r="I19" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J19" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K19" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L19" s="12" t="str">
         <f aca="false">I19&amp;"."&amp;J19&amp;"."&amp;K19</f>
-        <v>4.4.2022</v>
+        <v>7.6.2022</v>
       </c>
       <c r="M19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>26453</v>
+        <v>28324</v>
       </c>
       <c r="N19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>12574</v>
+        <v>10109</v>
       </c>
       <c r="O19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24141</v>
+        <v>4912</v>
       </c>
       <c r="P19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>421</v>
+        <v>26582</v>
       </c>
       <c r="Q19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4215</v>
+        <v>2715</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1187,38 +1187,38 @@
       </c>
       <c r="I20" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J20" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K20" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L20" s="12" t="str">
         <f aca="false">I20&amp;"."&amp;J20&amp;"."&amp;K20</f>
-        <v>7.7.2022</v>
+        <v>1.5.2022</v>
       </c>
       <c r="M20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>154</v>
+        <v>6584</v>
       </c>
       <c r="N20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4797</v>
+        <v>3247</v>
       </c>
       <c r="O20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2040</v>
+        <v>23672</v>
       </c>
       <c r="P20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22334</v>
+        <v>21411</v>
       </c>
       <c r="Q20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28304</v>
+        <v>26368</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1242,38 +1242,38 @@
       </c>
       <c r="I21" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J21" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="K21" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L21" s="12" t="str">
         <f aca="false">I21&amp;"."&amp;J21&amp;"."&amp;K21</f>
-        <v>1.8.2022</v>
+        <v>8.12.2022</v>
       </c>
       <c r="M21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3796</v>
+        <v>19284</v>
       </c>
       <c r="N21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>25114</v>
+        <v>27875</v>
       </c>
       <c r="O21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5054</v>
+        <v>21549</v>
       </c>
       <c r="P21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>25765</v>
+        <v>21858</v>
       </c>
       <c r="Q21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28803</v>
+        <v>17155</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="I22" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J22" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -1308,27 +1308,27 @@
       </c>
       <c r="L22" s="12" t="str">
         <f aca="false">I22&amp;"."&amp;J22&amp;"."&amp;K22</f>
-        <v>1.3.2022</v>
+        <v>6.3.2022</v>
       </c>
       <c r="M22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2531</v>
+        <v>14437</v>
       </c>
       <c r="N22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29473</v>
+        <v>15029</v>
       </c>
       <c r="O22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7467</v>
+        <v>24807</v>
       </c>
       <c r="P22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17726</v>
+        <v>9275</v>
       </c>
       <c r="Q22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23138</v>
+        <v>9039</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1352,38 +1352,38 @@
       </c>
       <c r="I23" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J23" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="K23" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L23" s="12" t="str">
         <f aca="false">I23&amp;"."&amp;J23&amp;"."&amp;K23</f>
-        <v>6.6.2022</v>
+        <v>9.12.2022</v>
       </c>
       <c r="M23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4931</v>
+        <v>5489</v>
       </c>
       <c r="N23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11894</v>
+        <v>18313</v>
       </c>
       <c r="O23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>14736</v>
+        <v>10205</v>
       </c>
       <c r="P23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19366</v>
+        <v>28043</v>
       </c>
       <c r="Q23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9190</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>